<commit_message>
Adding missing NIST 800-171 3.12.4 control
</commit_message>
<xml_diff>
--- a/Control Frameworks/NIST 800-171/NIST 800-171.xlsx
+++ b/Control Frameworks/NIST 800-171/NIST 800-171.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsokol/Documents/git/simplerisk/import-content/Control Frameworks/NIST 800-171/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E9280A-2F25-6D4E-9F4D-0FB43543E2B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C84F41-4EAE-3A4A-96E1-6F8BBE129AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="1120" windowWidth="32020" windowHeight="18640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="440" yWindow="500" windowWidth="32020" windowHeight="18640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NIST 800-171" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NIST 800-171'!$B$1:$L$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NIST 800-171'!$B$1:$L$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="534">
   <si>
     <t>NIST 800-53 Mapping</t>
   </si>
@@ -1617,6 +1624,29 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>3.12.4</t>
+  </si>
+  <si>
+    <t>System security plans relate security requirements to a set of security controls. System security plans also describe, at a high level, how the security controls meet those security requirements, but do not provide detailed, technical descriptions of the design or implementation of the controls.</t>
+  </si>
+  <si>
+    <t>NIST 800-53 Mapping: PL-2
+ISO 27002:2013 Mapping: A.6.1.2
+Relevant 20 Critial Control: N/A
+DFARS 7012 (2013) Covered: N/A</t>
+  </si>
+  <si>
+    <t>PL-2</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Develop, document, and periodically update system security plans that describe system
+boundaries, system environments of operation, how security requirements are implemented,
+and the relationships with or connections to other systems.</t>
   </si>
 </sst>
 </file>
@@ -2259,11 +2289,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AB965"/>
+  <dimension ref="A1:AB966"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E108" sqref="E108"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6345,18 +6375,18 @@
         <v>306</v>
       </c>
       <c r="E67" s="12" t="str">
-        <f t="shared" ref="E67:E110" si="3">_xlfn.CONCAT(A67, " ", B67)</f>
+        <f t="shared" ref="E67:E111" si="3">_xlfn.CONCAT(A67, " ", B67)</f>
         <v>NIST 800-171 3.8.3</v>
       </c>
       <c r="F67" s="12" t="str">
-        <f t="shared" ref="F67:F110" si="4">_xlfn.CONCAT(A67, " ", B67, ": ", M67)</f>
+        <f t="shared" ref="F67:F111" si="4">_xlfn.CONCAT(A67, " ", B67, ": ", M67)</f>
         <v>NIST 800-171 3.8.3: Sanitize or destroy information system media containing CUI before disposal or release for reuse.</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>317</v>
       </c>
       <c r="H67" s="12" t="str">
-        <f t="shared" ref="H67:H110" si="5">_xlfn.CONCAT("NIST 800-53 Mapping: ", I67, CHAR(10),CHAR(10),"ISO 27002:2013 Mapping: ", J67, CHAR(10),CHAR(10),"Relevant 20 Critical Control: ", K67, CHAR(10),CHAR(10),"DFARS 7012 (2013) Covered: ", L67)</f>
+        <f t="shared" ref="H67:H111" si="5">_xlfn.CONCAT("NIST 800-53 Mapping: ", I67, CHAR(10),CHAR(10),"ISO 27002:2013 Mapping: ", J67, CHAR(10),CHAR(10),"Relevant 20 Critical Control: ", K67, CHAR(10),CHAR(10),"DFARS 7012 (2013) Covered: ", L67)</f>
         <v>NIST 800-53 Mapping: MP-2, MP-4, MP-6
 ISO 27002:2013 Mapping: A.8.2.3, A.8.3.1, A.8.3.2, A.11.2.7, A.11.2.9
 Relevant 20 Critical Control: 8
@@ -7547,7 +7577,7 @@
       <c r="AA86" s="4"/>
       <c r="AB86" s="4"/>
     </row>
-    <row r="87" spans="1:28" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" ht="208" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
         <v>519</v>
       </c>
@@ -7609,51 +7639,49 @@
       <c r="AA87" s="4"/>
       <c r="AB87" s="4"/>
     </row>
-    <row r="88" spans="1:28" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" ht="128" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
         <v>519</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>409</v>
+        <v>528</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="E88" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.1</v>
+        <v>NIST 800-171 3.12.4</v>
       </c>
       <c r="F88" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.1: Monitor, control, and protect organizational communications (i.e., information transmitted or received by organizational information systems) at the external boundaries and key internal boundaries of the information systems.</v>
-      </c>
-      <c r="G88" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="H88" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-7, SA-8
-ISO 27002:2013 Mapping: A.8.2.3, A.13.1.1, A.13.1.3, A.13.2.1, A.13.2.3, A.14.1.2, A.14.1.3
-Relevant 20 Critical Control: 13, 19
-DFARS 7012 (2013) Covered: SC-7</v>
+        <v>NIST 800-171 3.12.4: Develop, document, and periodically update system security plans that describe system
+boundaries, system environments of operation, how security requirements are implemented,
+and the relationships with or connections to other systems.</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="H88" s="12" t="s">
+        <v>530</v>
       </c>
       <c r="I88" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="J88" s="6" t="s">
-        <v>414</v>
+        <v>531</v>
+      </c>
+      <c r="J88" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>415</v>
+        <v>532</v>
       </c>
       <c r="L88" s="6" t="s">
-        <v>416</v>
+        <v>532</v>
       </c>
       <c r="M88" s="6" t="s">
-        <v>411</v>
+        <v>533</v>
       </c>
       <c r="N88" s="4"/>
       <c r="O88" s="4"/>
@@ -7676,7 +7704,7 @@
         <v>519</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>5</v>
@@ -7686,19 +7714,19 @@
       </c>
       <c r="E89" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.2</v>
+        <v>NIST 800-171 3.13.1</v>
       </c>
       <c r="F89" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.2: Employ architectural designs, software development techniques, and systems engineering principles that promote effective information security within organizational information systems.</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>419</v>
+        <v>NIST 800-171 3.13.1: Monitor, control, and protect organizational communications (i.e., information transmitted or received by organizational information systems) at the external boundaries and key internal boundaries of the information systems.</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>412</v>
       </c>
       <c r="H89" s="12" t="str">
         <f t="shared" si="5"/>
         <v>NIST 800-53 Mapping: SC-7, SA-8
-ISO 27002:2013 Mapping: A.13.1.1, A.13.1.3, A.13.2.1, A.14.1.3, A.14.2.5
+ISO 27002:2013 Mapping: A.8.2.3, A.13.1.1, A.13.1.3, A.13.2.1, A.13.2.3, A.14.1.2, A.14.1.3
 Relevant 20 Critical Control: 13, 19
 DFARS 7012 (2013) Covered: SC-7</v>
       </c>
@@ -7706,7 +7734,7 @@
         <v>413</v>
       </c>
       <c r="J89" s="6" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="K89" s="6" t="s">
         <v>415</v>
@@ -7715,7 +7743,7 @@
         <v>416</v>
       </c>
       <c r="M89" s="6" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="N89" s="4"/>
       <c r="O89" s="4"/>
@@ -7738,44 +7766,46 @@
         <v>519</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>410</v>
       </c>
       <c r="E90" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.3</v>
+        <v>NIST 800-171 3.13.2</v>
       </c>
       <c r="F90" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.3: Separate user functionality from information system management functionality.</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>423</v>
+        <v>NIST 800-171 3.13.2: Employ architectural designs, software development techniques, and systems engineering principles that promote effective information security within organizational information systems.</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>419</v>
       </c>
       <c r="H90" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-2
-ISO 27002:2013 Mapping: None
-Relevant 20 Critical Control: 
-DFARS 7012 (2013) Covered: Yes</v>
+        <v>NIST 800-53 Mapping: SC-7, SA-8
+ISO 27002:2013 Mapping: A.13.1.1, A.13.1.3, A.13.2.1, A.14.1.3, A.14.2.5
+Relevant 20 Critical Control: 13, 19
+DFARS 7012 (2013) Covered: SC-7</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="J90" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K90" s="6"/>
+        <v>420</v>
+      </c>
+      <c r="K90" s="6" t="s">
+        <v>415</v>
+      </c>
       <c r="L90" s="6" t="s">
-        <v>24</v>
+        <v>416</v>
       </c>
       <c r="M90" s="6" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="N90" s="4"/>
       <c r="O90" s="4"/>
@@ -7798,7 +7828,7 @@
         <v>519</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>14</v>
@@ -7808,24 +7838,24 @@
       </c>
       <c r="E91" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.4</v>
+        <v>NIST 800-171 3.13.3</v>
       </c>
       <c r="F91" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.4: Prevent unauthorized and unintended information transfer via shared system resources.</v>
-      </c>
-      <c r="G91" s="6" t="s">
-        <v>427</v>
+        <v>NIST 800-171 3.13.3: Separate user functionality from information system management functionality.</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>423</v>
       </c>
       <c r="H91" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-4
+        <v>NIST 800-53 Mapping: SC-2
 ISO 27002:2013 Mapping: None
 Relevant 20 Critical Control: 
 DFARS 7012 (2013) Covered: Yes</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J91" s="6" t="s">
         <v>66</v>
@@ -7835,7 +7865,7 @@
         <v>24</v>
       </c>
       <c r="M91" s="6" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="N91" s="4"/>
       <c r="O91" s="4"/>
@@ -7858,7 +7888,7 @@
         <v>519</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>14</v>
@@ -7868,36 +7898,34 @@
       </c>
       <c r="E92" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.5</v>
+        <v>NIST 800-171 3.13.4</v>
       </c>
       <c r="F92" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.5: Implement subnetworks for publicly accessible system components that are physically or logically separated from internal networks.</v>
+        <v>NIST 800-171 3.13.4: Prevent unauthorized and unintended information transfer via shared system resources.</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="H92" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-7, SA-8
-ISO 27002:2013 Mapping: A.13.1.1, A.13.1.3, A.13.2.1, A.14.1.3, A.14.2.5
-Relevant 20 Critical Control: 13, 19
-DFARS 7012 (2013) Covered: SC-7</v>
+        <v>NIST 800-53 Mapping: SC-4
+ISO 27002:2013 Mapping: None
+Relevant 20 Critical Control: 
+DFARS 7012 (2013) Covered: Yes</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>413</v>
+        <v>428</v>
       </c>
       <c r="J92" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="K92" s="6" t="s">
-        <v>415</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="K92" s="6"/>
       <c r="L92" s="6" t="s">
-        <v>416</v>
+        <v>24</v>
       </c>
       <c r="M92" s="6" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="N92" s="4"/>
       <c r="O92" s="4"/>
@@ -7920,7 +7948,7 @@
         <v>519</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>14</v>
@@ -7930,36 +7958,36 @@
       </c>
       <c r="E93" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.6</v>
+        <v>NIST 800-171 3.13.5</v>
       </c>
       <c r="F93" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.6: Deny network communications traffic by default and allow network communications traffic by exception (i.e., deny all, permit by exception).</v>
+        <v>NIST 800-171 3.13.5: Implement subnetworks for publicly accessible system components that are physically or logically separated from internal networks.</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H93" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-7(5)
-ISO 27002:2013 Mapping: A.13.1.1, A.13.1.3, A.13.2.1, A.14.1.3
+        <v>NIST 800-53 Mapping: SC-7, SA-8
+ISO 27002:2013 Mapping: A.13.1.1, A.13.1.3, A.13.2.1, A.14.1.3, A.14.2.5
 Relevant 20 Critical Control: 13, 19
-DFARS 7012 (2013) Covered: No</v>
+DFARS 7012 (2013) Covered: SC-7</v>
       </c>
       <c r="I93" s="6" t="s">
-        <v>435</v>
+        <v>413</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="K93" s="6" t="s">
         <v>415</v>
       </c>
       <c r="L93" s="6" t="s">
-        <v>30</v>
+        <v>416</v>
       </c>
       <c r="M93" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="N93" s="4"/>
       <c r="O93" s="4"/>
@@ -7982,7 +8010,7 @@
         <v>519</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>14</v>
@@ -7992,24 +8020,24 @@
       </c>
       <c r="E94" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.7</v>
+        <v>NIST 800-171 3.13.6</v>
       </c>
       <c r="F94" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.7: Prevent remote devices from simultaneously establishing non-remote connections with the information system and communicating via some other connection to resources in external networks.</v>
+        <v>NIST 800-171 3.13.6: Deny network communications traffic by default and allow network communications traffic by exception (i.e., deny all, permit by exception).</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="H94" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-7(7)
+        <v>NIST 800-53 Mapping: SC-7(5)
 ISO 27002:2013 Mapping: A.13.1.1, A.13.1.3, A.13.2.1, A.14.1.3
 Relevant 20 Critical Control: 13, 19
 DFARS 7012 (2013) Covered: No</v>
       </c>
       <c r="I94" s="6" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="J94" s="6" t="s">
         <v>436</v>
@@ -8021,7 +8049,7 @@
         <v>30</v>
       </c>
       <c r="M94" s="6" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="N94" s="4"/>
       <c r="O94" s="4"/>
@@ -8044,7 +8072,7 @@
         <v>519</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>14</v>
@@ -8054,36 +8082,36 @@
       </c>
       <c r="E95" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.8</v>
+        <v>NIST 800-171 3.13.7</v>
       </c>
       <c r="F95" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.8: Implement cryptographic mechanisms to prevent unauthorized disclosure of CUI during transmission unless otherwise protected by alternative physical safeguards.</v>
+        <v>NIST 800-171 3.13.7: Prevent remote devices from simultaneously establishing non-remote connections with the information system and communicating via some other connection to resources in external networks.</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="H95" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-8, SC-8(1)
-ISO 27002:2013 Mapping: A.8.2.3, A.13.1.1, A.13.2.1, A.13.2.3, A.14.1.2, A.14.1.3
-Relevant 20 Critical Control: 17
-DFARS 7012 (2013) Covered: SC-8(1)</v>
+        <v>NIST 800-53 Mapping: SC-7(7)
+ISO 27002:2013 Mapping: A.13.1.1, A.13.1.3, A.13.2.1, A.14.1.3
+Relevant 20 Critical Control: 13, 19
+DFARS 7012 (2013) Covered: No</v>
       </c>
       <c r="I95" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="J95" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="K95" s="6">
-        <v>17</v>
+        <v>440</v>
+      </c>
+      <c r="J95" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>415</v>
       </c>
       <c r="L95" s="6" t="s">
-        <v>446</v>
+        <v>30</v>
       </c>
       <c r="M95" s="6" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
@@ -8106,7 +8134,7 @@
         <v>519</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>14</v>
@@ -8116,34 +8144,36 @@
       </c>
       <c r="E96" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.9</v>
+        <v>NIST 800-171 3.13.8</v>
       </c>
       <c r="F96" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.9: Terminate network connections associated with communications sessions at the end of the sessions or after a defined period of inactivity.</v>
+        <v>NIST 800-171 3.13.8: Implement cryptographic mechanisms to prevent unauthorized disclosure of CUI during transmission unless otherwise protected by alternative physical safeguards.</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="H96" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-10
-ISO 27002:2013 Mapping: A.13.1.1
-Relevant 20 Critical Control: 
-DFARS 7012 (2013) Covered: No</v>
+        <v>NIST 800-53 Mapping: SC-8, SC-8(1)
+ISO 27002:2013 Mapping: A.8.2.3, A.13.1.1, A.13.2.1, A.13.2.3, A.14.1.2, A.14.1.3
+Relevant 20 Critical Control: 17
+DFARS 7012 (2013) Covered: SC-8(1)</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="J96" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="K96" s="6"/>
+        <v>445</v>
+      </c>
+      <c r="K96" s="6">
+        <v>17</v>
+      </c>
       <c r="L96" s="6" t="s">
-        <v>30</v>
+        <v>446</v>
       </c>
       <c r="M96" s="6" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="N96" s="4"/>
       <c r="O96" s="4"/>
@@ -8166,7 +8196,7 @@
         <v>519</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>14</v>
@@ -8176,34 +8206,34 @@
       </c>
       <c r="E97" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.10</v>
+        <v>NIST 800-171 3.13.9</v>
       </c>
       <c r="F97" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.10: Establish and manage cryptographic keys for cryptography employed in the information system;</v>
-      </c>
-      <c r="G97" s="9" t="s">
-        <v>454</v>
+        <v>NIST 800-171 3.13.9: Terminate network connections associated with communications sessions at the end of the sessions or after a defined period of inactivity.</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>449</v>
       </c>
       <c r="H97" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-12
-ISO 27002:2013 Mapping: A.10.1.2
+        <v>NIST 800-53 Mapping: SC-10
+ISO 27002:2013 Mapping: A.13.1.1
 Relevant 20 Critical Control: 
 DFARS 7012 (2013) Covered: No</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="K97" s="6"/>
       <c r="L97" s="6" t="s">
         <v>30</v>
       </c>
       <c r="M97" s="6" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="N97" s="4"/>
       <c r="O97" s="4"/>
@@ -8226,7 +8256,7 @@
         <v>519</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>14</v>
@@ -8236,34 +8266,34 @@
       </c>
       <c r="E98" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.11</v>
+        <v>NIST 800-171 3.13.10</v>
       </c>
       <c r="F98" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.11: Employ FIPS-validated cryptography when used to protect the confidentiality of CUI.</v>
+        <v>NIST 800-171 3.13.10: Establish and manage cryptographic keys for cryptography employed in the information system;</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="H98" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-13
-ISO 27002:2013 Mapping: A.10.1.1, A.14.1.2, A.14.1.3, A.18.1.5
+        <v>NIST 800-53 Mapping: SC-12
+ISO 27002:2013 Mapping: A.10.1.2
 Relevant 20 Critical Control: 
-DFARS 7012 (2013) Covered: Yes</v>
+DFARS 7012 (2013) Covered: No</v>
       </c>
       <c r="I98" s="6" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="K98" s="6"/>
       <c r="L98" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="M98" s="6" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="N98" s="4"/>
       <c r="O98" s="4"/>
@@ -8286,7 +8316,7 @@
         <v>519</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>14</v>
@@ -8296,36 +8326,34 @@
       </c>
       <c r="E99" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.12</v>
+        <v>NIST 800-171 3.13.11</v>
       </c>
       <c r="F99" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.12: Prohibit remote activation of collaborative computing devices and provide indication of devices in use to users present at the device.</v>
+        <v>NIST 800-171 3.13.11: Employ FIPS-validated cryptography when used to protect the confidentiality of CUI.</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="H99" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-15
-ISO 27002:2013 Mapping: A.13.2.1 (ISO control doesn't completely match NIST 800-53)
-Relevant 20 Critical Control: 3
+        <v>NIST 800-53 Mapping: SC-13
+ISO 27002:2013 Mapping: A.10.1.1, A.14.1.2, A.14.1.3, A.18.1.5
+Relevant 20 Critical Control: 
 DFARS 7012 (2013) Covered: Yes</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="J99" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="K99" s="6">
-        <v>3</v>
-      </c>
+        <v>461</v>
+      </c>
+      <c r="K99" s="6"/>
       <c r="L99" s="6" t="s">
         <v>24</v>
       </c>
       <c r="M99" s="6" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="N99" s="4"/>
       <c r="O99" s="4"/>
@@ -8348,7 +8376,7 @@
         <v>519</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>14</v>
@@ -8358,36 +8386,36 @@
       </c>
       <c r="E100" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.13</v>
+        <v>NIST 800-171 3.13.12</v>
       </c>
       <c r="F100" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.13: Control and monitor the use of mobile code.</v>
+        <v>NIST 800-171 3.13.12: Prohibit remote activation of collaborative computing devices and provide indication of devices in use to users present at the device.</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="H100" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-18
-ISO 27002:2013 Mapping: None
-Relevant 20 Critical Control: 2
-DFARS 7012 (2013) Covered: No</v>
+        <v>NIST 800-53 Mapping: SC-15
+ISO 27002:2013 Mapping: A.13.2.1 (ISO control doesn't completely match NIST 800-53)
+Relevant 20 Critical Control: 3
+DFARS 7012 (2013) Covered: Yes</v>
       </c>
       <c r="I100" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="J100" s="6" t="s">
-        <v>66</v>
+        <v>465</v>
+      </c>
+      <c r="J100" s="7" t="s">
+        <v>466</v>
       </c>
       <c r="K100" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L100" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="M100" s="6" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="N100" s="4"/>
       <c r="O100" s="4"/>
@@ -8410,7 +8438,7 @@
         <v>519</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>14</v>
@@ -8420,34 +8448,36 @@
       </c>
       <c r="E101" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.14</v>
+        <v>NIST 800-171 3.13.13</v>
       </c>
       <c r="F101" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.14: Control and monitor the use of Voice over Internet Protocol (VoIP) technologies.</v>
+        <v>NIST 800-171 3.13.13: Control and monitor the use of mobile code.</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="H101" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-19
+        <v>NIST 800-53 Mapping: SC-18
 ISO 27002:2013 Mapping: None
-Relevant 20 Critical Control: 
+Relevant 20 Critical Control: 2
 DFARS 7012 (2013) Covered: No</v>
       </c>
       <c r="I101" s="6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="J101" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K101" s="6"/>
+      <c r="K101" s="6">
+        <v>2</v>
+      </c>
       <c r="L101" s="6" t="s">
         <v>30</v>
       </c>
       <c r="M101" s="6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="N101" s="4"/>
       <c r="O101" s="4"/>
@@ -8470,7 +8500,7 @@
         <v>519</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>14</v>
@@ -8480,36 +8510,34 @@
       </c>
       <c r="E102" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.15</v>
+        <v>NIST 800-171 3.13.14</v>
       </c>
       <c r="F102" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.15: Protect the authenticity of communications sessions.</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>477</v>
+        <v>NIST 800-171 3.13.14: Control and monitor the use of Voice over Internet Protocol (VoIP) technologies.</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>473</v>
       </c>
       <c r="H102" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-23
+        <v>NIST 800-53 Mapping: SC-19
 ISO 27002:2013 Mapping: None
-Relevant 20 Critical Control: 16
+Relevant 20 Critical Control: 
 DFARS 7012 (2013) Covered: No</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="J102" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K102" s="6">
-        <v>16</v>
-      </c>
+      <c r="K102" s="6"/>
       <c r="L102" s="6" t="s">
         <v>30</v>
       </c>
       <c r="M102" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="N102" s="4"/>
       <c r="O102" s="4"/>
@@ -8532,7 +8560,7 @@
         <v>519</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>14</v>
@@ -8542,36 +8570,36 @@
       </c>
       <c r="E103" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.13.16</v>
+        <v>NIST 800-171 3.13.15</v>
       </c>
       <c r="F103" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.13.16: Protect the confidentiality of CUI at rest.</v>
+        <v>NIST 800-171 3.13.15: Protect the authenticity of communications sessions.</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="H103" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SC-28
-ISO 27002:2013 Mapping: A.8.2.3 (ISO control doesn't completely match NIST 800-53)
-Relevant 20 Critical Control: 17
-DFARS 7012 (2013) Covered: Yes</v>
+        <v>NIST 800-53 Mapping: SC-23
+ISO 27002:2013 Mapping: None
+Relevant 20 Critical Control: 16
+DFARS 7012 (2013) Covered: No</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>483</v>
+        <v>66</v>
       </c>
       <c r="K103" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L103" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="M103" s="6" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="N103" s="4"/>
       <c r="O103" s="4"/>
@@ -8594,46 +8622,46 @@
         <v>519</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>485</v>
+        <v>410</v>
       </c>
       <c r="E104" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.14.1</v>
+        <v>NIST 800-171 3.13.16</v>
       </c>
       <c r="F104" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.14.1: Identify, report, and correct information and information system flaws in a timely manner.</v>
+        <v>NIST 800-171 3.13.16: Protect the confidentiality of CUI at rest.</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="H104" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SI-2, SI-3, SI-5
-ISO 27002:2013 Mapping: A.6.1.4 (ISO control doesn't completely match NIST 800-53), A.12.2.1, A.12.6.1, A.14.2.2, A.14.2.3, A.16.1.3
-Relevant 20 Critical Control: 3, 5
-DFARS 7012 (2013) Covered: SI-2, SI-3</v>
+        <v>NIST 800-53 Mapping: SC-28
+ISO 27002:2013 Mapping: A.8.2.3 (ISO control doesn't completely match NIST 800-53)
+Relevant 20 Critical Control: 17
+DFARS 7012 (2013) Covered: Yes</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="J104" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="K104" s="6" t="s">
-        <v>490</v>
+        <v>483</v>
+      </c>
+      <c r="K104" s="6">
+        <v>17</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>491</v>
+        <v>24</v>
       </c>
       <c r="M104" s="6" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="N104" s="4"/>
       <c r="O104" s="4"/>
@@ -8656,7 +8684,7 @@
         <v>519</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>5</v>
@@ -8666,14 +8694,14 @@
       </c>
       <c r="E105" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.14.2</v>
+        <v>NIST 800-171 3.14.1</v>
       </c>
       <c r="F105" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.14.2: Provide protection from malicious code at appropriate locations within organizational information systems.</v>
+        <v>NIST 800-171 3.14.1: Identify, report, and correct information and information system flaws in a timely manner.</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="H105" s="12" t="str">
         <f t="shared" si="5"/>
@@ -8695,7 +8723,7 @@
         <v>491</v>
       </c>
       <c r="M105" s="6" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="N105" s="4"/>
       <c r="O105" s="4"/>
@@ -8718,7 +8746,7 @@
         <v>519</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>5</v>
@@ -8728,14 +8756,14 @@
       </c>
       <c r="E106" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.14.3</v>
+        <v>NIST 800-171 3.14.2</v>
       </c>
       <c r="F106" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.14.3: Monitor information system security alerts and advisories and take appropriate actions in response.</v>
+        <v>NIST 800-171 3.14.2: Provide protection from malicious code at appropriate locations within organizational information systems.</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H106" s="12" t="str">
         <f t="shared" si="5"/>
@@ -8757,7 +8785,7 @@
         <v>491</v>
       </c>
       <c r="M106" s="6" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="N106" s="4"/>
       <c r="O106" s="4"/>
@@ -8780,46 +8808,46 @@
         <v>519</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>485</v>
       </c>
       <c r="E107" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.14.4</v>
+        <v>NIST 800-171 3.14.3</v>
       </c>
       <c r="F107" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.14.4: Update malicious code protection mechanisms when new releases are available.</v>
+        <v>NIST 800-171 3.14.3: Monitor information system security alerts and advisories and take appropriate actions in response.</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="H107" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SI-3
-ISO 27002:2013 Mapping: A.12.2.1
-Relevant 20 Critical Control: 5
-DFARS 7012 (2013) Covered: Yes</v>
+        <v>NIST 800-53 Mapping: SI-2, SI-3, SI-5
+ISO 27002:2013 Mapping: A.6.1.4 (ISO control doesn't completely match NIST 800-53), A.12.2.1, A.12.6.1, A.14.2.2, A.14.2.3, A.16.1.3
+Relevant 20 Critical Control: 3, 5
+DFARS 7012 (2013) Covered: SI-2, SI-3</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="J107" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="K107" s="6">
-        <v>5</v>
+        <v>488</v>
+      </c>
+      <c r="J107" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="K107" s="6" t="s">
+        <v>490</v>
       </c>
       <c r="L107" s="6" t="s">
-        <v>24</v>
+        <v>491</v>
       </c>
       <c r="M107" s="6" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="N107" s="4"/>
       <c r="O107" s="4"/>
@@ -8842,7 +8870,7 @@
         <v>519</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>14</v>
@@ -8852,14 +8880,14 @@
       </c>
       <c r="E108" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.14.5</v>
+        <v>NIST 800-171 3.14.4</v>
       </c>
       <c r="F108" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.14.5: Perform periodic scans of the information system and real-time scans of files from external sources as files are downloaded, opened, or executed.</v>
+        <v>NIST 800-171 3.14.4: Update malicious code protection mechanisms when new releases are available.</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="H108" s="12" t="str">
         <f t="shared" si="5"/>
@@ -8881,7 +8909,7 @@
         <v>24</v>
       </c>
       <c r="M108" s="6" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="N108" s="4"/>
       <c r="O108" s="4"/>
@@ -8904,7 +8932,7 @@
         <v>519</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>14</v>
@@ -8914,36 +8942,36 @@
       </c>
       <c r="E109" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.14.6</v>
+        <v>NIST 800-171 3.14.5</v>
       </c>
       <c r="F109" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.14.6: Monitor the information system including inbound and outbound communications traffic, to detect attacks and indicators of potential attacks.</v>
+        <v>NIST 800-171 3.14.5: Perform periodic scans of the information system and real-time scans of files from external sources as files are downloaded, opened, or executed.</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="H109" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SI-4, SI-4(4)
-ISO 27002:2013 Mapping: None
-Relevant 20 Critical Control: 1, 2, 3, 5, 7, 10, 11, 12, 13, 14, 15, 16, 17, 
-DFARS 7012 (2013) Covered: SI-4</v>
+        <v>NIST 800-53 Mapping: SI-3
+ISO 27002:2013 Mapping: A.12.2.1
+Relevant 20 Critical Control: 5
+DFARS 7012 (2013) Covered: Yes</v>
       </c>
       <c r="I109" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="J109" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K109" s="6" t="s">
-        <v>510</v>
+        <v>501</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="K109" s="6">
+        <v>5</v>
       </c>
       <c r="L109" s="6" t="s">
-        <v>511</v>
+        <v>24</v>
       </c>
       <c r="M109" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="N109" s="4"/>
       <c r="O109" s="4"/>
@@ -8966,7 +8994,7 @@
         <v>519</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>14</v>
@@ -8976,36 +9004,36 @@
       </c>
       <c r="E110" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>NIST 800-171 3.14.7</v>
+        <v>NIST 800-171 3.14.6</v>
       </c>
       <c r="F110" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>NIST 800-171 3.14.7: Identify unauthorized use of the information system.</v>
+        <v>NIST 800-171 3.14.6: Monitor the information system including inbound and outbound communications traffic, to detect attacks and indicators of potential attacks.</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="H110" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>NIST 800-53 Mapping: SI-4
+        <v>NIST 800-53 Mapping: SI-4, SI-4(4)
 ISO 27002:2013 Mapping: None
-Relevant 20 Critical Control: 1, 2, 3, 5, 7, 10, 11, 12, 13, 14, 15, 16, 17
-DFARS 7012 (2013) Covered: Yes</v>
+Relevant 20 Critical Control: 1, 2, 3, 5, 7, 10, 11, 12, 13, 14, 15, 16, 17, 
+DFARS 7012 (2013) Covered: SI-4</v>
       </c>
       <c r="I110" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J110" s="6" t="s">
         <v>66</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>24</v>
+        <v>511</v>
       </c>
       <c r="M110" s="6" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="N110" s="4"/>
       <c r="O110" s="4"/>
@@ -9023,17 +9051,52 @@
       <c r="AA110" s="4"/>
       <c r="AB110" s="4"/>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
-      <c r="H111" s="1"/>
-      <c r="I111" s="1"/>
-      <c r="J111" s="1"/>
-      <c r="K111" s="1"/>
-      <c r="L111" s="1"/>
-      <c r="M111" s="1"/>
+    <row r="111" spans="1:28" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="E111" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>NIST 800-171 3.14.7</v>
+      </c>
+      <c r="F111" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>NIST 800-171 3.14.7: Identify unauthorized use of the information system.</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="H111" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NIST 800-53 Mapping: SI-4
+ISO 27002:2013 Mapping: None
+Relevant 20 Critical Control: 1, 2, 3, 5, 7, 10, 11, 12, 13, 14, 15, 16, 17
+DFARS 7012 (2013) Covered: Yes</v>
+      </c>
+      <c r="I111" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="J111" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K111" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="L111" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M111" s="6" t="s">
+        <v>513</v>
+      </c>
       <c r="N111" s="4"/>
       <c r="O111" s="4"/>
       <c r="P111" s="4"/>
@@ -32108,8 +32171,35 @@
       <c r="AA965" s="4"/>
       <c r="AB965" s="4"/>
     </row>
+    <row r="966" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D966" s="1"/>
+      <c r="E966" s="1"/>
+      <c r="F966" s="1"/>
+      <c r="G966" s="1"/>
+      <c r="H966" s="1"/>
+      <c r="I966" s="1"/>
+      <c r="J966" s="1"/>
+      <c r="K966" s="1"/>
+      <c r="L966" s="1"/>
+      <c r="M966" s="1"/>
+      <c r="N966" s="4"/>
+      <c r="O966" s="4"/>
+      <c r="P966" s="4"/>
+      <c r="Q966" s="4"/>
+      <c r="R966" s="4"/>
+      <c r="S966" s="4"/>
+      <c r="T966" s="4"/>
+      <c r="U966" s="4"/>
+      <c r="V966" s="4"/>
+      <c r="W966" s="4"/>
+      <c r="X966" s="4"/>
+      <c r="Y966" s="4"/>
+      <c r="Z966" s="4"/>
+      <c r="AA966" s="4"/>
+      <c r="AB966" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:L110" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B1:L111" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="K82">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">

</xml_diff>